<commit_message>
ultimo aggiornamento file excel
</commit_message>
<xml_diff>
--- a/PaolaLucci/BilancioFamiliare/Progetto Python.xlsx
+++ b/PaolaLucci/BilancioFamiliare/Progetto Python.xlsx
@@ -1161,45 +1161,18 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="5" fillId="4" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="7" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="6" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="6" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="8" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="9" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1211,17 +1184,8 @@
     <xf numFmtId="4" fontId="6" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="5" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1237,15 +1201,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1307,11 +1262,76 @@
     <xf numFmtId="1" fontId="6" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="5" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="19">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1374,11 +1394,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1394,31 +1414,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1806,7 +1806,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="UCGUniCredit" id="{FEC4543A-5506-46B6-BB43-9DC5518B395B}" vid="{8BD5B8CA-27DC-4788-BE41-A870883ABEDB}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="UCGUniCredit" id="{FEC4543A-5506-46B6-BB43-9DC5518B395B}" vid="{8BD5B8CA-27DC-4788-BE41-A870883ABEDB}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2325,17 +2325,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" style="43" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" style="43" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="44"/>
-    <col min="4" max="5" width="8.140625" style="44" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="14.7109375" style="44" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" style="31" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="31" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="32"/>
+    <col min="4" max="5" width="8.140625" style="32" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14.7109375" style="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -2354,452 +2354,491 @@
       <c r="G1" s="9"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="101" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="11">
         <f>'Mese 1'!C4</f>
         <v>2000</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="11">
         <f>'Mese 2'!C4</f>
         <v>1950</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
+      <c r="E2" s="11">
+        <f>'Mese 3'!C4</f>
+        <v>1850</v>
+      </c>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="13"/>
-      <c r="B3" s="11" t="s">
+      <c r="A3" s="102"/>
+      <c r="B3" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="13"/>
-      <c r="B4" s="11" t="s">
+      <c r="A4" s="102"/>
+      <c r="B4" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="11">
         <f>'Mese 1'!C10</f>
         <v>3.54</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
-      <c r="B5" s="11" t="s">
+      <c r="A5" s="102"/>
+      <c r="B5" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="13"/>
-      <c r="B6" s="14" t="s">
+      <c r="A6" s="102"/>
+      <c r="B6" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="13"/>
-      <c r="B7" s="14" t="s">
+      <c r="A7" s="102"/>
+      <c r="B7" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="13"/>
-      <c r="B8" s="14" t="s">
+      <c r="A8" s="102"/>
+      <c r="B8" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="13"/>
-      <c r="B9" s="11" t="s">
+      <c r="A9" s="102"/>
+      <c r="B9" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="14" t="s">
+      <c r="A10" s="102"/>
+      <c r="B10" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
     </row>
     <row r="11" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="15" t="s">
+      <c r="A11" s="102"/>
+      <c r="B11" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="14">
         <f>SUM(C2:C9)</f>
         <v>2003.54</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="14">
         <f>SUM(D2:D9)</f>
         <v>1950</v>
       </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
+      <c r="E11" s="14">
+        <f>SUM(E2:E10)</f>
+        <v>1850</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="13"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
+      <c r="A12" s="102"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="13" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="18" t="s">
+      <c r="A13" s="103"/>
+      <c r="B13" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="16">
         <f>'Mese 1'!F3</f>
         <v>117</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="16">
         <f>('Mese 2'!F3+'Mese 1'!F39)</f>
         <v>162.5</v>
       </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
+      <c r="E13" s="16">
+        <f>'Mese 3'!F3</f>
+        <v>104</v>
+      </c>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="20"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
     </row>
     <row r="15" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="104" t="s">
         <v>93</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="C16" s="23">
+      <c r="C16" s="19">
         <f>'Mese 1'!G39</f>
         <v>1269.8599999999999</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="19">
         <f>'Mese 2'!G33</f>
         <v>1481.9099999999999</v>
       </c>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
+      <c r="E16" s="19">
+        <f>'Mese 3'!G36</f>
+        <v>1425.81</v>
+      </c>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
     </row>
     <row r="17" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
+      <c r="A17" s="105"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
-      <c r="B18" s="25" t="s">
+      <c r="A18" s="105"/>
+      <c r="B18" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="C18" s="26">
+      <c r="C18" s="21">
         <f>C16</f>
         <v>1269.8599999999999</v>
       </c>
-      <c r="D18" s="26">
-        <f>D16</f>
+      <c r="D18" s="21">
+        <f t="shared" ref="D18:E18" si="0">D16</f>
         <v>1481.9099999999999</v>
       </c>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
+      <c r="E18" s="21">
+        <f t="shared" si="0"/>
+        <v>1425.81</v>
+      </c>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="24"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
+      <c r="A19" s="105"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
     </row>
     <row r="20" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
-      <c r="B20" s="18" t="s">
+      <c r="A20" s="106"/>
+      <c r="B20" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="16">
         <f>SUM('Mese 1'!F4:F38)</f>
         <v>84.5</v>
       </c>
-      <c r="D20" s="19">
+      <c r="D20" s="16">
         <f>SUM('Mese 2'!F4:F32)</f>
         <v>91</v>
       </c>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
+      <c r="E20" s="16">
+        <f>SUM('Mese 3'!F4:F32)</f>
+        <v>45.5</v>
+      </c>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="20"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
     </row>
     <row r="22" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="110" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="C23" s="23">
+      <c r="C23" s="19">
         <f>'Mese 1'!J39</f>
         <v>250</v>
       </c>
-      <c r="D23" s="23">
+      <c r="D23" s="19">
         <f>'Mese 2'!J33</f>
         <v>250</v>
       </c>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
+      <c r="E23" s="19">
+        <f>'Mese 3'!J36</f>
+        <v>250</v>
+      </c>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
     </row>
     <row r="24" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
+      <c r="A24" s="111"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
-      <c r="B25" s="31" t="s">
+      <c r="A25" s="112"/>
+      <c r="B25" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="C25" s="32">
+      <c r="C25" s="23">
         <f>C23</f>
         <v>250</v>
       </c>
-      <c r="D25" s="32">
+      <c r="D25" s="23">
         <f>D23</f>
         <v>250</v>
       </c>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
+      <c r="E25" s="23">
+        <f>E23</f>
+        <v>250</v>
+      </c>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="20"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
     </row>
     <row r="27" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
+      <c r="A27" s="17"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
     </row>
     <row r="28" spans="1:7" s="7" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="33" t="s">
+      <c r="A28" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="B28" s="34" t="s">
+      <c r="B28" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="C28" s="35">
+      <c r="C28" s="26">
         <f>'Mese 1'!H39</f>
         <v>375.46</v>
       </c>
-      <c r="D28" s="35">
+      <c r="D28" s="26">
         <f>'Mese 2'!H33</f>
         <v>49</v>
       </c>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
+      <c r="E28" s="26">
+        <f>'Mese 3'!H36</f>
+        <v>474</v>
+      </c>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="20"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
+      <c r="A29" s="17"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
     </row>
     <row r="30" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
+      <c r="A30" s="17"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="36" t="s">
+      <c r="A31" s="107" t="s">
         <v>106</v>
       </c>
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C31" s="23">
+      <c r="C31" s="19">
         <f>C2*0.1</f>
         <v>200</v>
       </c>
-      <c r="D31" s="23">
+      <c r="D31" s="19">
         <f>D2*0.1</f>
         <v>195</v>
       </c>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
+      <c r="E31" s="19">
+        <f>E2*0.1</f>
+        <v>185</v>
+      </c>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="37"/>
-      <c r="B32" s="11" t="s">
+      <c r="A32" s="108"/>
+      <c r="B32" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C32" s="12">
+      <c r="C32" s="11">
         <f>'Mese 1'!F39</f>
         <v>32.5</v>
       </c>
-      <c r="D32" s="12">
+      <c r="D32" s="11">
         <f>D13-D20</f>
         <v>71.5</v>
       </c>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
+      <c r="E32" s="11">
+        <f>'Mese 3'!O2</f>
+        <v>91</v>
+      </c>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
     </row>
     <row r="33" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="37"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
+      <c r="A33" s="108"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
     </row>
     <row r="34" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="37"/>
-      <c r="B34" s="38" t="s">
+      <c r="A34" s="108"/>
+      <c r="B34" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C34" s="39">
+      <c r="C34" s="28">
         <f>C11-C18-C25</f>
         <v>483.68000000000006</v>
       </c>
-      <c r="D34" s="39">
+      <c r="D34" s="28">
         <f>D11-D18-D25</f>
         <v>218.09000000000015</v>
       </c>
-      <c r="E34" s="39"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="39"/>
+      <c r="E34" s="28">
+        <f>E11-E18-E25</f>
+        <v>174.19000000000005</v>
+      </c>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="37"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
+      <c r="A35" s="108"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
     </row>
     <row r="36" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="40"/>
-      <c r="B36" s="41" t="s">
+      <c r="A36" s="109"/>
+      <c r="B36" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="C36" s="42">
+      <c r="C36" s="30">
         <f>C34-C31</f>
         <v>283.68000000000006</v>
       </c>
-      <c r="D36" s="42">
+      <c r="D36" s="30">
         <f>D34-D31</f>
         <v>23.090000000000146</v>
       </c>
-      <c r="E36" s="42"/>
-      <c r="F36" s="42"/>
-      <c r="G36" s="42"/>
+      <c r="E36" s="30">
+        <f>E34-E31</f>
+        <v>-10.809999999999945</v>
+      </c>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2808,27 +2847,27 @@
     <mergeCell ref="A31:A36"/>
     <mergeCell ref="A23:A25"/>
   </mergeCells>
-  <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="15" priority="4" operator="greaterThan">
+  <conditionalFormatting sqref="C34 E34">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="greaterThan">
       <formula>$C$31</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="greaterThan">
       <formula>$C$31</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="greaterThan">
       <formula>$D$31</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F34:G34">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
       <formula>$D$31</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
-      <formula>$D$31</formula>
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>$E$31</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2840,801 +2879,801 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36:G37"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="43" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" style="43" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="43" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="43" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" style="43" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" style="43" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="43" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" style="43" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" style="43" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" style="43" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6" style="43" customWidth="1"/>
-    <col min="12" max="12" width="27.85546875" style="43" customWidth="1"/>
-    <col min="13" max="15" width="9.28515625" style="43" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" style="31" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="31" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="31" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" style="31" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6" style="31" customWidth="1"/>
+    <col min="12" max="12" width="27.85546875" style="31" customWidth="1"/>
+    <col min="13" max="15" width="9.28515625" style="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="48"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="50" t="s">
+      <c r="E1" s="36"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="51"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="53" t="s">
+      <c r="H1" s="39"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="54" t="s">
+      <c r="L1" s="113" t="s">
         <v>78</v>
       </c>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="56"/>
+      <c r="M1" s="114"/>
+      <c r="N1" s="114"/>
+      <c r="O1" s="115"/>
     </row>
     <row r="2" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="57"/>
-      <c r="B2" s="58"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="57" t="s">
+      <c r="A2" s="42"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="60" t="s">
+      <c r="E2" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="61" t="s">
+      <c r="F2" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="63" t="s">
+      <c r="H2" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="64" t="s">
+      <c r="I2" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="J2" s="65"/>
-      <c r="L2" s="57" t="s">
+      <c r="J2" s="50"/>
+      <c r="L2" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="M2" s="115">
+      <c r="M2" s="100">
         <f>D39</f>
         <v>5</v>
       </c>
-      <c r="N2" s="66">
+      <c r="N2" s="51"/>
+      <c r="O2" s="52">
         <f>F3-SUM(F4:F38)</f>
         <v>32.5</v>
       </c>
-      <c r="O2" s="67"/>
     </row>
     <row r="3" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="68"/>
-      <c r="B3" s="69"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="71">
+      <c r="A3" s="53"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="56">
         <v>18</v>
       </c>
-      <c r="E3" s="72">
+      <c r="E3" s="57">
         <v>6.5</v>
       </c>
-      <c r="F3" s="73">
+      <c r="F3" s="58">
         <f>D3*E3</f>
         <v>117</v>
       </c>
-      <c r="G3" s="74"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="77"/>
-      <c r="L3" s="74" t="s">
+      <c r="G3" s="59"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="62"/>
+      <c r="L3" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="M3" s="75"/>
-      <c r="N3" s="78"/>
-      <c r="O3" s="79">
+      <c r="M3" s="60"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="64">
         <f>C39*0.1</f>
         <v>200.35400000000001</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="80">
+      <c r="A4" s="65">
         <v>44953</v>
       </c>
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="81">
+      <c r="C4" s="66">
         <v>2000</v>
       </c>
-      <c r="D4" s="111"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="87"/>
-      <c r="J4" s="88"/>
-      <c r="L4" s="68" t="s">
+      <c r="D4" s="96"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="73"/>
+      <c r="L4" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="M4" s="89"/>
-      <c r="N4" s="69"/>
-      <c r="O4" s="90">
+      <c r="M4" s="74"/>
+      <c r="N4" s="54"/>
+      <c r="O4" s="75">
         <f>G39</f>
         <v>1269.8599999999999</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="80"/>
-      <c r="B5" s="69" t="s">
+      <c r="A5" s="65"/>
+      <c r="B5" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="81"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="85">
+      <c r="C5" s="66"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="70">
         <v>39.9</v>
       </c>
-      <c r="H5" s="86"/>
-      <c r="I5" s="87"/>
-      <c r="J5" s="88"/>
-      <c r="L5" s="91" t="s">
+      <c r="H5" s="71"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="73"/>
+      <c r="L5" s="76" t="s">
         <v>80</v>
       </c>
-      <c r="M5" s="89"/>
-      <c r="N5" s="69"/>
-      <c r="O5" s="90">
+      <c r="M5" s="74"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="75">
         <f>H39</f>
         <v>375.46</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="80">
+      <c r="A6" s="65">
         <v>44954</v>
       </c>
-      <c r="B6" s="69" t="s">
+      <c r="B6" s="54" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="81"/>
-      <c r="D6" s="112"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="85">
+      <c r="C6" s="66"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="70">
         <v>27</v>
       </c>
-      <c r="H6" s="86"/>
-      <c r="I6" s="87"/>
-      <c r="J6" s="88"/>
-      <c r="L6" s="68" t="s">
+      <c r="H6" s="71"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="73"/>
+      <c r="L6" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="89"/>
-      <c r="N6" s="69"/>
-      <c r="O6" s="90">
+      <c r="M6" s="74"/>
+      <c r="N6" s="54"/>
+      <c r="O6" s="75">
         <f>J39</f>
         <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="80">
+      <c r="A7" s="65">
         <v>44955</v>
       </c>
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="C7" s="81"/>
-      <c r="D7" s="112"/>
-      <c r="E7" s="86"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="85"/>
-      <c r="H7" s="86"/>
-      <c r="I7" s="87">
+      <c r="C7" s="66"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="71"/>
+      <c r="I7" s="72">
         <v>95</v>
       </c>
-      <c r="J7" s="88"/>
-      <c r="L7" s="92" t="s">
+      <c r="J7" s="73"/>
+      <c r="L7" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="M7" s="93"/>
-      <c r="N7" s="94"/>
-      <c r="O7" s="95">
+      <c r="M7" s="78"/>
+      <c r="N7" s="79"/>
+      <c r="O7" s="80">
         <f>C39-G39-J39</f>
         <v>483.68000000000006</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="80">
+      <c r="A8" s="65">
         <v>44956</v>
       </c>
-      <c r="B8" s="69"/>
-      <c r="C8" s="81"/>
-      <c r="D8" s="112"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="87"/>
-      <c r="G8" s="85"/>
-      <c r="H8" s="86"/>
-      <c r="I8" s="87"/>
-      <c r="J8" s="88"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="73"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="80">
+      <c r="A9" s="65">
         <v>44957</v>
       </c>
-      <c r="B9" s="69" t="s">
+      <c r="B9" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="81"/>
-      <c r="D9" s="112"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="87"/>
-      <c r="G9" s="85">
+      <c r="C9" s="66"/>
+      <c r="D9" s="97"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="70">
         <v>500</v>
       </c>
-      <c r="H9" s="86"/>
-      <c r="I9" s="87"/>
-      <c r="J9" s="88"/>
-      <c r="L9" s="43" t="s">
+      <c r="H9" s="71"/>
+      <c r="I9" s="72"/>
+      <c r="J9" s="73"/>
+      <c r="L9" s="31" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="80"/>
-      <c r="B10" s="69" t="s">
+      <c r="A10" s="65"/>
+      <c r="B10" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="81">
+      <c r="C10" s="66">
         <v>3.54</v>
       </c>
-      <c r="D10" s="112"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="87"/>
-      <c r="G10" s="85"/>
-      <c r="H10" s="86"/>
-      <c r="I10" s="87"/>
-      <c r="J10" s="88"/>
+      <c r="D10" s="97"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="70"/>
+      <c r="H10" s="71"/>
+      <c r="I10" s="72"/>
+      <c r="J10" s="73"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="80">
+      <c r="A11" s="65">
         <v>44958</v>
       </c>
-      <c r="B11" s="69" t="s">
+      <c r="B11" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="81"/>
-      <c r="D11" s="112"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="87"/>
-      <c r="G11" s="85">
+      <c r="C11" s="66"/>
+      <c r="D11" s="97"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="72"/>
+      <c r="G11" s="70">
         <v>70</v>
       </c>
-      <c r="H11" s="86"/>
-      <c r="I11" s="87"/>
-      <c r="J11" s="88"/>
+      <c r="H11" s="71"/>
+      <c r="I11" s="72"/>
+      <c r="J11" s="73"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="80">
+      <c r="A12" s="65">
         <v>44959</v>
       </c>
-      <c r="B12" s="69" t="s">
+      <c r="B12" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="81"/>
-      <c r="D12" s="112"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="87"/>
-      <c r="G12" s="85">
+      <c r="C12" s="66"/>
+      <c r="D12" s="97"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="72"/>
+      <c r="G12" s="70">
         <v>25</v>
       </c>
-      <c r="H12" s="86"/>
-      <c r="I12" s="87"/>
-      <c r="J12" s="88"/>
+      <c r="H12" s="71"/>
+      <c r="I12" s="72"/>
+      <c r="J12" s="73"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="80">
+      <c r="A13" s="65">
         <v>44960</v>
       </c>
-      <c r="B13" s="69"/>
-      <c r="C13" s="81"/>
-      <c r="D13" s="112"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="87"/>
-      <c r="G13" s="85"/>
-      <c r="H13" s="86"/>
-      <c r="I13" s="87"/>
-      <c r="J13" s="88"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="97"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="70"/>
+      <c r="H13" s="71"/>
+      <c r="I13" s="72"/>
+      <c r="J13" s="73"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="80">
+      <c r="A14" s="65">
         <v>44961</v>
       </c>
-      <c r="B14" s="69" t="s">
+      <c r="B14" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="81"/>
-      <c r="D14" s="112"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="87"/>
-      <c r="G14" s="85">
+      <c r="C14" s="66"/>
+      <c r="D14" s="97"/>
+      <c r="E14" s="71"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="70">
         <v>11.92</v>
       </c>
-      <c r="H14" s="86"/>
-      <c r="I14" s="87"/>
-      <c r="J14" s="88"/>
+      <c r="H14" s="71"/>
+      <c r="I14" s="72"/>
+      <c r="J14" s="73"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="80">
+      <c r="A15" s="65">
         <v>44962</v>
       </c>
-      <c r="B15" s="69" t="s">
+      <c r="B15" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="81"/>
-      <c r="D15" s="112">
+      <c r="C15" s="66"/>
+      <c r="D15" s="97">
         <v>8</v>
       </c>
-      <c r="E15" s="86">
+      <c r="E15" s="71">
         <v>6.5</v>
       </c>
-      <c r="F15" s="87">
+      <c r="F15" s="72">
         <f>D15*E15</f>
         <v>52</v>
       </c>
-      <c r="G15" s="85">
+      <c r="G15" s="70">
         <v>10.56</v>
       </c>
-      <c r="H15" s="86"/>
-      <c r="I15" s="87"/>
-      <c r="J15" s="88"/>
+      <c r="H15" s="71"/>
+      <c r="I15" s="72"/>
+      <c r="J15" s="73"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="80"/>
-      <c r="B16" s="69" t="s">
+      <c r="A16" s="65"/>
+      <c r="B16" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="81"/>
-      <c r="D16" s="112"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="87"/>
-      <c r="G16" s="85"/>
-      <c r="H16" s="86"/>
-      <c r="I16" s="87"/>
-      <c r="J16" s="88">
+      <c r="C16" s="66"/>
+      <c r="D16" s="97"/>
+      <c r="E16" s="71"/>
+      <c r="F16" s="72"/>
+      <c r="G16" s="70"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="72"/>
+      <c r="J16" s="73">
         <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="80">
+      <c r="A17" s="65">
         <v>44963</v>
       </c>
-      <c r="B17" s="69"/>
-      <c r="C17" s="81"/>
-      <c r="D17" s="112"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="87"/>
-      <c r="G17" s="85"/>
-      <c r="H17" s="86"/>
-      <c r="I17" s="87"/>
-      <c r="J17" s="88"/>
+      <c r="B17" s="54"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="97"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="72"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="72"/>
+      <c r="J17" s="73"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="80">
+      <c r="A18" s="65">
         <v>44964</v>
       </c>
-      <c r="B18" s="69" t="s">
+      <c r="B18" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="C18" s="81"/>
-      <c r="D18" s="112"/>
-      <c r="E18" s="86"/>
-      <c r="F18" s="87"/>
-      <c r="G18" s="85">
+      <c r="C18" s="66"/>
+      <c r="D18" s="97"/>
+      <c r="E18" s="71"/>
+      <c r="F18" s="72"/>
+      <c r="G18" s="70">
         <v>47</v>
       </c>
-      <c r="H18" s="86"/>
-      <c r="I18" s="87"/>
-      <c r="J18" s="88"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="72"/>
+      <c r="J18" s="73"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="80">
+      <c r="A19" s="65">
         <v>44965</v>
       </c>
-      <c r="B19" s="69"/>
-      <c r="C19" s="81"/>
-      <c r="D19" s="112"/>
-      <c r="E19" s="86"/>
-      <c r="F19" s="87"/>
-      <c r="G19" s="85"/>
-      <c r="H19" s="86"/>
-      <c r="I19" s="87"/>
-      <c r="J19" s="88"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="97"/>
+      <c r="E19" s="71"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="70"/>
+      <c r="H19" s="71"/>
+      <c r="I19" s="72"/>
+      <c r="J19" s="73"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="80">
+      <c r="A20" s="65">
         <v>44966</v>
       </c>
-      <c r="B20" s="69" t="s">
+      <c r="B20" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="81"/>
-      <c r="D20" s="112"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="87"/>
-      <c r="G20" s="85">
+      <c r="C20" s="66"/>
+      <c r="D20" s="97"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="72"/>
+      <c r="G20" s="70">
         <v>26</v>
       </c>
-      <c r="H20" s="86"/>
-      <c r="I20" s="87"/>
-      <c r="J20" s="88"/>
+      <c r="H20" s="71"/>
+      <c r="I20" s="72"/>
+      <c r="J20" s="73"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="80">
+      <c r="A21" s="65">
         <v>44967</v>
       </c>
-      <c r="B21" s="69" t="s">
+      <c r="B21" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="81"/>
-      <c r="D21" s="112"/>
-      <c r="E21" s="86"/>
-      <c r="F21" s="87"/>
-      <c r="G21" s="85">
+      <c r="C21" s="66"/>
+      <c r="D21" s="97"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="70">
         <v>217</v>
       </c>
-      <c r="H21" s="86"/>
-      <c r="I21" s="87"/>
-      <c r="J21" s="88"/>
+      <c r="H21" s="71"/>
+      <c r="I21" s="72"/>
+      <c r="J21" s="73"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="80">
+      <c r="A22" s="65">
         <v>44968</v>
       </c>
-      <c r="B22" s="69" t="s">
+      <c r="B22" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="81"/>
-      <c r="D22" s="112"/>
-      <c r="E22" s="86"/>
-      <c r="F22" s="87"/>
-      <c r="G22" s="85"/>
-      <c r="H22" s="86">
+      <c r="C22" s="66"/>
+      <c r="D22" s="97"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="70"/>
+      <c r="H22" s="71">
         <v>375.46</v>
       </c>
-      <c r="I22" s="87"/>
-      <c r="J22" s="88"/>
+      <c r="I22" s="72"/>
+      <c r="J22" s="73"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="80">
+      <c r="A23" s="65">
         <v>44969</v>
       </c>
-      <c r="B23" s="69"/>
-      <c r="C23" s="81"/>
-      <c r="D23" s="112"/>
-      <c r="E23" s="86"/>
-      <c r="F23" s="87"/>
-      <c r="G23" s="85"/>
-      <c r="H23" s="86"/>
-      <c r="I23" s="87"/>
-      <c r="J23" s="88"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="97"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="72"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="71"/>
+      <c r="I23" s="72"/>
+      <c r="J23" s="73"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="80">
+      <c r="A24" s="65">
         <v>44970</v>
       </c>
-      <c r="B24" s="69"/>
-      <c r="C24" s="81"/>
-      <c r="D24" s="112"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="87"/>
-      <c r="G24" s="85"/>
-      <c r="H24" s="86"/>
-      <c r="I24" s="87"/>
-      <c r="J24" s="88"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="66"/>
+      <c r="D24" s="97"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="72"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="72"/>
+      <c r="J24" s="73"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="80">
+      <c r="A25" s="65">
         <v>44971</v>
       </c>
-      <c r="B25" s="69" t="s">
+      <c r="B25" s="54" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="81"/>
-      <c r="D25" s="112"/>
-      <c r="E25" s="86"/>
-      <c r="F25" s="87"/>
-      <c r="G25" s="85">
+      <c r="C25" s="66"/>
+      <c r="D25" s="97"/>
+      <c r="E25" s="71"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="70">
         <v>32</v>
       </c>
-      <c r="H25" s="86"/>
-      <c r="I25" s="87"/>
-      <c r="J25" s="88"/>
+      <c r="H25" s="71"/>
+      <c r="I25" s="72"/>
+      <c r="J25" s="73"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="80">
+      <c r="A26" s="65">
         <v>44972</v>
       </c>
-      <c r="B26" s="69" t="s">
+      <c r="B26" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="C26" s="81"/>
-      <c r="D26" s="112"/>
-      <c r="E26" s="86"/>
-      <c r="F26" s="87"/>
-      <c r="G26" s="85">
+      <c r="C26" s="66"/>
+      <c r="D26" s="97"/>
+      <c r="E26" s="71"/>
+      <c r="F26" s="72"/>
+      <c r="G26" s="70">
         <v>13</v>
       </c>
-      <c r="H26" s="86"/>
-      <c r="I26" s="87"/>
-      <c r="J26" s="88"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="72"/>
+      <c r="J26" s="73"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="80">
+      <c r="A27" s="65">
         <v>44973</v>
       </c>
-      <c r="B27" s="69" t="s">
+      <c r="B27" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="81"/>
-      <c r="D27" s="112"/>
-      <c r="E27" s="86"/>
-      <c r="F27" s="87"/>
-      <c r="G27" s="85">
+      <c r="C27" s="66"/>
+      <c r="D27" s="97"/>
+      <c r="E27" s="71"/>
+      <c r="F27" s="72"/>
+      <c r="G27" s="70">
         <v>18</v>
       </c>
-      <c r="H27" s="86"/>
-      <c r="I27" s="87"/>
-      <c r="J27" s="88"/>
+      <c r="H27" s="71"/>
+      <c r="I27" s="72"/>
+      <c r="J27" s="73"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="80">
+      <c r="A28" s="65">
         <v>44974</v>
       </c>
-      <c r="B28" s="69"/>
-      <c r="C28" s="81"/>
-      <c r="D28" s="112"/>
-      <c r="E28" s="86"/>
-      <c r="F28" s="87"/>
-      <c r="G28" s="85"/>
-      <c r="H28" s="86"/>
-      <c r="I28" s="87"/>
-      <c r="J28" s="88"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="97"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="72"/>
+      <c r="G28" s="70"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="72"/>
+      <c r="J28" s="73"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="80">
+      <c r="A29" s="65">
         <v>44975</v>
       </c>
-      <c r="B29" s="69" t="s">
+      <c r="B29" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="81"/>
-      <c r="D29" s="112">
+      <c r="C29" s="66"/>
+      <c r="D29" s="97">
         <v>5</v>
       </c>
-      <c r="E29" s="86">
+      <c r="E29" s="71">
         <v>6.5</v>
       </c>
-      <c r="F29" s="87">
+      <c r="F29" s="72">
         <f>D29*E29</f>
         <v>32.5</v>
       </c>
-      <c r="G29" s="85"/>
-      <c r="H29" s="86"/>
-      <c r="I29" s="87"/>
-      <c r="J29" s="88"/>
+      <c r="G29" s="70"/>
+      <c r="H29" s="71"/>
+      <c r="I29" s="72"/>
+      <c r="J29" s="73"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="80">
+      <c r="A30" s="65">
         <v>44976</v>
       </c>
-      <c r="B30" s="69"/>
-      <c r="C30" s="81"/>
-      <c r="D30" s="112"/>
-      <c r="E30" s="86"/>
-      <c r="F30" s="87"/>
-      <c r="G30" s="85"/>
-      <c r="H30" s="86"/>
-      <c r="I30" s="87"/>
-      <c r="J30" s="88"/>
+      <c r="B30" s="54"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="97"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="72"/>
+      <c r="G30" s="70"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="72"/>
+      <c r="J30" s="73"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="80">
+      <c r="A31" s="65">
         <v>44977</v>
       </c>
-      <c r="B31" s="69" t="s">
+      <c r="B31" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="81"/>
-      <c r="D31" s="112"/>
-      <c r="E31" s="86"/>
-      <c r="F31" s="87"/>
-      <c r="G31" s="85"/>
-      <c r="H31" s="86"/>
-      <c r="I31" s="87"/>
-      <c r="J31" s="88">
+      <c r="C31" s="66"/>
+      <c r="D31" s="97"/>
+      <c r="E31" s="71"/>
+      <c r="F31" s="72"/>
+      <c r="G31" s="70"/>
+      <c r="H31" s="71"/>
+      <c r="I31" s="72"/>
+      <c r="J31" s="73">
         <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="80">
+      <c r="A32" s="65">
         <v>44978</v>
       </c>
-      <c r="B32" s="69"/>
-      <c r="C32" s="81"/>
-      <c r="D32" s="112"/>
-      <c r="E32" s="86"/>
-      <c r="F32" s="87"/>
-      <c r="G32" s="85"/>
-      <c r="H32" s="86"/>
-      <c r="I32" s="87"/>
-      <c r="J32" s="88"/>
+      <c r="B32" s="54"/>
+      <c r="C32" s="66"/>
+      <c r="D32" s="97"/>
+      <c r="E32" s="71"/>
+      <c r="F32" s="72"/>
+      <c r="G32" s="70"/>
+      <c r="H32" s="71"/>
+      <c r="I32" s="72"/>
+      <c r="J32" s="73"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A33" s="80">
+      <c r="A33" s="65">
         <v>44979</v>
       </c>
-      <c r="B33" s="69" t="s">
+      <c r="B33" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="C33" s="81"/>
-      <c r="D33" s="112"/>
-      <c r="E33" s="86"/>
-      <c r="F33" s="87"/>
-      <c r="G33" s="85">
+      <c r="C33" s="66"/>
+      <c r="D33" s="97"/>
+      <c r="E33" s="71"/>
+      <c r="F33" s="72"/>
+      <c r="G33" s="70">
         <v>25</v>
       </c>
-      <c r="H33" s="86"/>
-      <c r="I33" s="87"/>
-      <c r="J33" s="88"/>
+      <c r="H33" s="71"/>
+      <c r="I33" s="72"/>
+      <c r="J33" s="73"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A34" s="80">
+      <c r="A34" s="65">
         <v>44980</v>
       </c>
-      <c r="B34" s="69" t="s">
+      <c r="B34" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="81"/>
-      <c r="D34" s="112"/>
-      <c r="E34" s="86"/>
-      <c r="F34" s="87"/>
-      <c r="G34" s="85">
+      <c r="C34" s="66"/>
+      <c r="D34" s="97"/>
+      <c r="E34" s="71"/>
+      <c r="F34" s="72"/>
+      <c r="G34" s="70">
         <v>30</v>
       </c>
-      <c r="H34" s="86"/>
-      <c r="I34" s="87"/>
-      <c r="J34" s="88"/>
+      <c r="H34" s="71"/>
+      <c r="I34" s="72"/>
+      <c r="J34" s="73"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A35" s="80">
+      <c r="A35" s="65">
         <v>44981</v>
       </c>
-      <c r="B35" s="69" t="s">
+      <c r="B35" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="C35" s="81"/>
-      <c r="D35" s="112"/>
-      <c r="E35" s="86"/>
-      <c r="F35" s="87"/>
-      <c r="G35" s="85">
+      <c r="C35" s="66"/>
+      <c r="D35" s="97"/>
+      <c r="E35" s="71"/>
+      <c r="F35" s="72"/>
+      <c r="G35" s="70">
         <v>16</v>
       </c>
-      <c r="H35" s="86"/>
-      <c r="I35" s="87"/>
-      <c r="J35" s="88"/>
+      <c r="H35" s="71"/>
+      <c r="I35" s="72"/>
+      <c r="J35" s="73"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A36" s="80">
+      <c r="A36" s="65">
         <v>44982</v>
       </c>
-      <c r="B36" s="69" t="s">
+      <c r="B36" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="C36" s="81"/>
-      <c r="D36" s="112"/>
-      <c r="E36" s="86"/>
-      <c r="F36" s="87"/>
-      <c r="G36" s="85">
+      <c r="C36" s="66"/>
+      <c r="D36" s="97"/>
+      <c r="E36" s="71"/>
+      <c r="F36" s="72"/>
+      <c r="G36" s="70">
         <v>96.08</v>
       </c>
-      <c r="H36" s="86"/>
-      <c r="I36" s="87"/>
-      <c r="J36" s="88"/>
+      <c r="H36" s="71"/>
+      <c r="I36" s="72"/>
+      <c r="J36" s="73"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A37" s="80"/>
-      <c r="B37" s="69" t="s">
+      <c r="A37" s="65"/>
+      <c r="B37" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="C37" s="81"/>
-      <c r="D37" s="112"/>
-      <c r="E37" s="86"/>
-      <c r="F37" s="87"/>
-      <c r="G37" s="85">
+      <c r="C37" s="66"/>
+      <c r="D37" s="97"/>
+      <c r="E37" s="71"/>
+      <c r="F37" s="72"/>
+      <c r="G37" s="70">
         <v>65.400000000000006</v>
       </c>
-      <c r="H37" s="86"/>
-      <c r="I37" s="87"/>
-      <c r="J37" s="88"/>
+      <c r="H37" s="71"/>
+      <c r="I37" s="72"/>
+      <c r="J37" s="73"/>
     </row>
     <row r="38" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="96">
+      <c r="A38" s="81">
         <v>44983</v>
       </c>
-      <c r="B38" s="97"/>
-      <c r="C38" s="98"/>
-      <c r="D38" s="113"/>
-      <c r="E38" s="100"/>
-      <c r="F38" s="101"/>
-      <c r="G38" s="99"/>
-      <c r="H38" s="100"/>
-      <c r="I38" s="101"/>
-      <c r="J38" s="102"/>
+      <c r="B38" s="82"/>
+      <c r="C38" s="83"/>
+      <c r="D38" s="98"/>
+      <c r="E38" s="85"/>
+      <c r="F38" s="86"/>
+      <c r="G38" s="84"/>
+      <c r="H38" s="85"/>
+      <c r="I38" s="86"/>
+      <c r="J38" s="87"/>
     </row>
     <row r="39" spans="1:15" s="6" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="103"/>
-      <c r="B39" s="104"/>
-      <c r="C39" s="105">
+      <c r="A39" s="88"/>
+      <c r="B39" s="89"/>
+      <c r="C39" s="90">
         <f>SUM(C4:C38)</f>
         <v>2003.54</v>
       </c>
-      <c r="D39" s="114">
+      <c r="D39" s="99">
         <f>D3-SUM(D4:D38)</f>
         <v>5</v>
       </c>
-      <c r="E39" s="107"/>
-      <c r="F39" s="108">
+      <c r="E39" s="92"/>
+      <c r="F39" s="93">
         <f>F3-SUM(F4:F38)</f>
         <v>32.5</v>
       </c>
-      <c r="G39" s="106">
+      <c r="G39" s="91">
         <f>SUM(G4:G38)</f>
         <v>1269.8599999999999</v>
       </c>
-      <c r="H39" s="107">
+      <c r="H39" s="92">
         <f>SUM(H4:H38)</f>
         <v>375.46</v>
       </c>
-      <c r="I39" s="108">
+      <c r="I39" s="93">
         <f>SUM(I7:I38)</f>
         <v>95</v>
       </c>
-      <c r="J39" s="109">
+      <c r="J39" s="94">
         <f>SUM(J4:J38)</f>
         <v>250</v>
       </c>
-      <c r="K39" s="110"/>
-      <c r="L39" s="110"/>
-      <c r="M39" s="110"/>
-      <c r="N39" s="110"/>
-      <c r="O39" s="110"/>
+      <c r="K39" s="95"/>
+      <c r="L39" s="95"/>
+      <c r="M39" s="95"/>
+      <c r="N39" s="95"/>
+      <c r="O39" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="L1:O1"/>
   </mergeCells>
   <conditionalFormatting sqref="O7">
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="greaterThan">
       <formula>$O$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="greaterThan">
       <formula>$O$3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3647,690 +3686,690 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="43" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" style="43" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="9.28515625" style="43" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" style="43" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="43" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" style="43" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" style="43" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" style="43" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="43"/>
-    <col min="12" max="12" width="26.85546875" style="43" customWidth="1"/>
-    <col min="13" max="15" width="9.28515625" style="43" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="9.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="31"/>
+    <col min="12" max="12" width="26.85546875" style="31" customWidth="1"/>
+    <col min="13" max="15" width="9.28515625" style="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="48"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="50" t="s">
+      <c r="E1" s="36"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="51"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="53" t="s">
+      <c r="H1" s="39"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="54" t="s">
+      <c r="L1" s="113" t="s">
         <v>78</v>
       </c>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="56"/>
+      <c r="M1" s="114"/>
+      <c r="N1" s="114"/>
+      <c r="O1" s="115"/>
     </row>
     <row r="2" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="57"/>
-      <c r="B2" s="58"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="57" t="s">
+      <c r="A2" s="42"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="60" t="s">
+      <c r="E2" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="61" t="s">
+      <c r="F2" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="63" t="s">
+      <c r="H2" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="64" t="s">
+      <c r="I2" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="J2" s="65"/>
-      <c r="L2" s="57" t="s">
+      <c r="J2" s="50"/>
+      <c r="L2" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="M2" s="115">
+      <c r="M2" s="100">
         <f>D3-(SUM(D4:D32))+'Mese 1'!M2</f>
         <v>11</v>
       </c>
-      <c r="N2" s="66">
+      <c r="N2" s="51"/>
+      <c r="O2" s="52">
         <f>'Mese 1'!F39+F3-(SUM(F4:F32))</f>
         <v>71.5</v>
       </c>
-      <c r="O2" s="67"/>
     </row>
     <row r="3" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="68"/>
-      <c r="B3" s="69"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="71">
+      <c r="A3" s="53"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="56">
         <v>20</v>
       </c>
-      <c r="E3" s="72">
+      <c r="E3" s="57">
         <v>6.5</v>
       </c>
-      <c r="F3" s="73">
+      <c r="F3" s="58">
         <f>D3*E3</f>
         <v>130</v>
       </c>
-      <c r="G3" s="74"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="77"/>
-      <c r="L3" s="74" t="s">
+      <c r="G3" s="59"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="62"/>
+      <c r="L3" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="M3" s="75"/>
-      <c r="N3" s="78"/>
-      <c r="O3" s="79">
+      <c r="M3" s="60"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="64">
         <f>C33*0.1</f>
         <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="80">
+      <c r="A4" s="65">
         <v>44984</v>
       </c>
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="81">
+      <c r="C4" s="66">
         <v>1950</v>
       </c>
-      <c r="D4" s="82"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="87"/>
-      <c r="J4" s="88"/>
-      <c r="L4" s="68" t="s">
+      <c r="D4" s="67"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="73"/>
+      <c r="L4" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="M4" s="89"/>
-      <c r="N4" s="69"/>
-      <c r="O4" s="90">
+      <c r="M4" s="74"/>
+      <c r="N4" s="54"/>
+      <c r="O4" s="75">
         <f>G33</f>
         <v>1481.9099999999999</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="80"/>
-      <c r="B5" s="69" t="s">
+      <c r="A5" s="65"/>
+      <c r="B5" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="81"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="85">
+      <c r="C5" s="66"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="70">
         <v>39.9</v>
       </c>
-      <c r="H5" s="86"/>
-      <c r="I5" s="87"/>
-      <c r="J5" s="88"/>
-      <c r="L5" s="68" t="s">
+      <c r="H5" s="71"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="73"/>
+      <c r="L5" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="M5" s="89"/>
-      <c r="N5" s="69"/>
-      <c r="O5" s="90">
+      <c r="M5" s="74"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="75">
         <f>H33</f>
         <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="80">
+      <c r="A6" s="65">
         <v>44985</v>
       </c>
-      <c r="B6" s="69" t="s">
+      <c r="B6" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="81"/>
-      <c r="D6" s="85"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="85">
+      <c r="C6" s="66"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="70">
         <v>500</v>
       </c>
-      <c r="H6" s="86"/>
-      <c r="I6" s="87"/>
-      <c r="J6" s="88"/>
-      <c r="L6" s="68" t="s">
+      <c r="H6" s="71"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="73"/>
+      <c r="L6" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="89"/>
-      <c r="N6" s="69"/>
-      <c r="O6" s="90">
+      <c r="M6" s="74"/>
+      <c r="N6" s="54"/>
+      <c r="O6" s="75">
         <f>J33</f>
         <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="80">
+      <c r="A7" s="65">
         <v>44986</v>
       </c>
-      <c r="B7" s="69"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="85"/>
-      <c r="E7" s="86"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="85"/>
-      <c r="H7" s="86"/>
-      <c r="I7" s="87"/>
-      <c r="J7" s="88"/>
-      <c r="L7" s="92" t="s">
+      <c r="B7" s="54"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="71"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="73"/>
+      <c r="L7" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="M7" s="93"/>
-      <c r="N7" s="94"/>
-      <c r="O7" s="95">
+      <c r="M7" s="78"/>
+      <c r="N7" s="79"/>
+      <c r="O7" s="80">
         <f>C33-G33-J33</f>
         <v>218.09000000000015</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="80">
+      <c r="A8" s="65">
         <v>44987</v>
       </c>
-      <c r="B8" s="69" t="s">
+      <c r="B8" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="81"/>
-      <c r="D8" s="85"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="87"/>
-      <c r="G8" s="85">
+      <c r="C8" s="66"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="70">
         <v>48.14</v>
       </c>
-      <c r="H8" s="86"/>
-      <c r="I8" s="87"/>
-      <c r="J8" s="88"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="73"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="80">
+      <c r="A9" s="65">
         <v>44988</v>
       </c>
-      <c r="B9" s="69" t="s">
+      <c r="B9" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="81"/>
-      <c r="D9" s="85"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="87"/>
-      <c r="G9" s="85">
+      <c r="C9" s="66"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="70">
         <v>40</v>
       </c>
-      <c r="H9" s="86"/>
-      <c r="I9" s="87"/>
-      <c r="J9" s="88"/>
-      <c r="L9" s="43" t="s">
+      <c r="H9" s="71"/>
+      <c r="I9" s="72"/>
+      <c r="J9" s="73"/>
+      <c r="L9" s="31" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="80">
+      <c r="A10" s="65">
         <v>44989</v>
       </c>
-      <c r="B10" s="69" t="s">
+      <c r="B10" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="81"/>
-      <c r="D10" s="85"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="87"/>
-      <c r="G10" s="85">
+      <c r="C10" s="66"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="70">
         <v>11.92</v>
       </c>
-      <c r="H10" s="86"/>
-      <c r="I10" s="87"/>
-      <c r="J10" s="88"/>
+      <c r="H10" s="71"/>
+      <c r="I10" s="72"/>
+      <c r="J10" s="73"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="80">
+      <c r="A11" s="65">
         <v>44990</v>
       </c>
-      <c r="B11" s="69" t="s">
+      <c r="B11" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="81"/>
-      <c r="D11" s="85"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="87"/>
-      <c r="G11" s="85"/>
-      <c r="H11" s="86"/>
-      <c r="I11" s="87"/>
-      <c r="J11" s="88">
+      <c r="C11" s="66"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="72"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="71"/>
+      <c r="I11" s="72"/>
+      <c r="J11" s="73">
         <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="80">
+      <c r="A12" s="65">
         <v>44991</v>
       </c>
-      <c r="B12" s="69" t="s">
+      <c r="B12" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="81"/>
-      <c r="D12" s="85"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="87"/>
-      <c r="G12" s="85">
+      <c r="C12" s="66"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="72"/>
+      <c r="G12" s="70">
         <v>47</v>
       </c>
-      <c r="H12" s="86"/>
-      <c r="I12" s="87"/>
-      <c r="J12" s="88"/>
+      <c r="H12" s="71"/>
+      <c r="I12" s="72"/>
+      <c r="J12" s="73"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="80">
+      <c r="A13" s="65">
         <v>44992</v>
       </c>
-      <c r="B13" s="69" t="s">
+      <c r="B13" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="81"/>
-      <c r="D13" s="85"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="87"/>
-      <c r="G13" s="85">
+      <c r="C13" s="66"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="70">
         <v>25</v>
       </c>
-      <c r="H13" s="86"/>
-      <c r="I13" s="87"/>
-      <c r="J13" s="88"/>
+      <c r="H13" s="71"/>
+      <c r="I13" s="72"/>
+      <c r="J13" s="73"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="80">
+      <c r="A14" s="65">
         <v>44993</v>
       </c>
-      <c r="B14" s="69" t="s">
+      <c r="B14" s="54" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="81"/>
-      <c r="D14" s="85"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="87"/>
-      <c r="G14" s="85">
+      <c r="C14" s="66"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="71"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="70">
         <v>80</v>
       </c>
-      <c r="H14" s="86"/>
-      <c r="I14" s="87"/>
-      <c r="J14" s="88"/>
+      <c r="H14" s="71"/>
+      <c r="I14" s="72"/>
+      <c r="J14" s="73"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="80">
+      <c r="A15" s="65">
         <v>44994</v>
       </c>
-      <c r="B15" s="69"/>
-      <c r="C15" s="81"/>
-      <c r="D15" s="85"/>
-      <c r="E15" s="86"/>
-      <c r="F15" s="87"/>
-      <c r="G15" s="85"/>
-      <c r="H15" s="86"/>
-      <c r="I15" s="87"/>
-      <c r="J15" s="88"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="71"/>
+      <c r="F15" s="72"/>
+      <c r="G15" s="70"/>
+      <c r="H15" s="71"/>
+      <c r="I15" s="72"/>
+      <c r="J15" s="73"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="80">
+      <c r="A16" s="65">
         <v>44995</v>
       </c>
-      <c r="B16" s="69" t="s">
+      <c r="B16" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="C16" s="81"/>
-      <c r="D16" s="85"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="87"/>
-      <c r="G16" s="85">
+      <c r="C16" s="66"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="71"/>
+      <c r="F16" s="72"/>
+      <c r="G16" s="70">
         <f>'Mese 1'!O5</f>
         <v>375.46</v>
       </c>
-      <c r="H16" s="86"/>
-      <c r="I16" s="87"/>
-      <c r="J16" s="88"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="72"/>
+      <c r="J16" s="73"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="80">
+      <c r="A17" s="65">
         <v>44996</v>
       </c>
-      <c r="B17" s="69" t="s">
+      <c r="B17" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="81"/>
-      <c r="D17" s="85">
+      <c r="C17" s="66"/>
+      <c r="D17" s="70">
         <v>8</v>
       </c>
-      <c r="E17" s="86">
+      <c r="E17" s="71">
         <v>6.5</v>
       </c>
-      <c r="F17" s="87">
+      <c r="F17" s="72">
         <f>D17*E17</f>
         <v>52</v>
       </c>
-      <c r="G17" s="85">
+      <c r="G17" s="70">
         <v>1.65</v>
       </c>
-      <c r="H17" s="86"/>
-      <c r="I17" s="87"/>
-      <c r="J17" s="88"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="72"/>
+      <c r="J17" s="73"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="80">
+      <c r="A18" s="65">
         <v>44997</v>
       </c>
-      <c r="B18" s="69"/>
-      <c r="C18" s="81"/>
-      <c r="D18" s="85"/>
-      <c r="E18" s="86"/>
-      <c r="F18" s="87"/>
-      <c r="G18" s="85"/>
-      <c r="H18" s="86"/>
-      <c r="I18" s="87"/>
-      <c r="J18" s="88"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="71"/>
+      <c r="F18" s="72"/>
+      <c r="G18" s="70"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="72"/>
+      <c r="J18" s="73"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="80">
+      <c r="A19" s="65">
         <v>44998</v>
       </c>
-      <c r="B19" s="69" t="s">
+      <c r="B19" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="81"/>
-      <c r="D19" s="85"/>
-      <c r="E19" s="86"/>
-      <c r="F19" s="87"/>
-      <c r="G19" s="85">
+      <c r="C19" s="66"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="71"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="70">
         <v>5</v>
       </c>
-      <c r="H19" s="86"/>
-      <c r="I19" s="87"/>
-      <c r="J19" s="88"/>
+      <c r="H19" s="71"/>
+      <c r="I19" s="72"/>
+      <c r="J19" s="73"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="80">
+      <c r="A20" s="65">
         <v>44999</v>
       </c>
-      <c r="B20" s="69"/>
-      <c r="C20" s="81"/>
-      <c r="D20" s="85"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="87"/>
-      <c r="G20" s="85"/>
-      <c r="H20" s="86"/>
-      <c r="I20" s="87"/>
-      <c r="J20" s="88"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="66"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="72"/>
+      <c r="G20" s="70"/>
+      <c r="H20" s="71"/>
+      <c r="I20" s="72"/>
+      <c r="J20" s="73"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="80">
+      <c r="A21" s="65">
         <v>45000</v>
       </c>
-      <c r="B21" s="69" t="s">
+      <c r="B21" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="81"/>
-      <c r="D21" s="85"/>
-      <c r="E21" s="86"/>
-      <c r="F21" s="87"/>
-      <c r="G21" s="85">
+      <c r="C21" s="66"/>
+      <c r="D21" s="70"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="70">
         <v>26</v>
       </c>
-      <c r="H21" s="86"/>
-      <c r="I21" s="87"/>
-      <c r="J21" s="88"/>
+      <c r="H21" s="71"/>
+      <c r="I21" s="72"/>
+      <c r="J21" s="73"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="80">
+      <c r="A22" s="65">
         <v>45001</v>
       </c>
-      <c r="B22" s="69" t="s">
+      <c r="B22" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="C22" s="81"/>
-      <c r="D22" s="85"/>
-      <c r="E22" s="86"/>
-      <c r="F22" s="87"/>
-      <c r="G22" s="85">
+      <c r="C22" s="66"/>
+      <c r="D22" s="70"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="70">
         <v>217</v>
       </c>
-      <c r="H22" s="86"/>
-      <c r="I22" s="87"/>
-      <c r="J22" s="88"/>
+      <c r="H22" s="71"/>
+      <c r="I22" s="72"/>
+      <c r="J22" s="73"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="80">
+      <c r="A23" s="65">
         <v>45002</v>
       </c>
-      <c r="B23" s="69"/>
-      <c r="C23" s="81"/>
-      <c r="D23" s="85"/>
-      <c r="E23" s="86"/>
-      <c r="F23" s="87"/>
-      <c r="G23" s="85"/>
-      <c r="H23" s="86"/>
-      <c r="I23" s="87"/>
-      <c r="J23" s="88"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="70"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="72"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="71"/>
+      <c r="I23" s="72"/>
+      <c r="J23" s="73"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="80">
+      <c r="A24" s="65">
         <v>45003</v>
       </c>
-      <c r="B24" s="69" t="s">
+      <c r="B24" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="81"/>
-      <c r="D24" s="85"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="87"/>
-      <c r="G24" s="85"/>
-      <c r="H24" s="86">
+      <c r="C24" s="66"/>
+      <c r="D24" s="70"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="72"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="71">
         <v>49</v>
       </c>
-      <c r="I24" s="87"/>
-      <c r="J24" s="88"/>
+      <c r="I24" s="72"/>
+      <c r="J24" s="73"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="80">
+      <c r="A25" s="65">
         <v>45004</v>
       </c>
-      <c r="B25" s="69"/>
-      <c r="C25" s="81"/>
-      <c r="D25" s="85"/>
-      <c r="E25" s="86"/>
-      <c r="F25" s="87"/>
-      <c r="G25" s="85"/>
-      <c r="H25" s="86"/>
-      <c r="I25" s="87"/>
-      <c r="J25" s="88"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="66"/>
+      <c r="D25" s="70"/>
+      <c r="E25" s="71"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="70"/>
+      <c r="H25" s="71"/>
+      <c r="I25" s="72"/>
+      <c r="J25" s="73"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="80">
+      <c r="A26" s="65">
         <v>45005</v>
       </c>
-      <c r="B26" s="69" t="s">
+      <c r="B26" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="81"/>
-      <c r="D26" s="85"/>
-      <c r="E26" s="86"/>
-      <c r="F26" s="87"/>
-      <c r="G26" s="85"/>
-      <c r="H26" s="86"/>
-      <c r="I26" s="87"/>
-      <c r="J26" s="88">
+      <c r="C26" s="66"/>
+      <c r="D26" s="70"/>
+      <c r="E26" s="71"/>
+      <c r="F26" s="72"/>
+      <c r="G26" s="70"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="72"/>
+      <c r="J26" s="73">
         <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="80">
+      <c r="A27" s="65">
         <v>45006</v>
       </c>
-      <c r="B27" s="69" t="s">
+      <c r="B27" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="81"/>
-      <c r="D27" s="85"/>
-      <c r="E27" s="86"/>
-      <c r="F27" s="87"/>
-      <c r="G27" s="85">
+      <c r="C27" s="66"/>
+      <c r="D27" s="70"/>
+      <c r="E27" s="71"/>
+      <c r="F27" s="72"/>
+      <c r="G27" s="70">
         <v>40</v>
       </c>
-      <c r="H27" s="86"/>
-      <c r="I27" s="87"/>
-      <c r="J27" s="88"/>
+      <c r="H27" s="71"/>
+      <c r="I27" s="72"/>
+      <c r="J27" s="73"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="80">
+      <c r="A28" s="65">
         <v>45007</v>
       </c>
-      <c r="B28" s="69" t="s">
+      <c r="B28" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="81"/>
-      <c r="D28" s="85"/>
-      <c r="E28" s="86"/>
-      <c r="F28" s="87"/>
-      <c r="G28" s="85">
+      <c r="C28" s="66"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="72"/>
+      <c r="G28" s="70">
         <v>18</v>
       </c>
-      <c r="H28" s="86"/>
-      <c r="I28" s="87"/>
-      <c r="J28" s="88"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="72"/>
+      <c r="J28" s="73"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="80">
+      <c r="A29" s="65">
         <v>45008</v>
       </c>
-      <c r="B29" s="69"/>
-      <c r="C29" s="81"/>
-      <c r="D29" s="85"/>
-      <c r="E29" s="86"/>
-      <c r="F29" s="87"/>
-      <c r="G29" s="85"/>
-      <c r="H29" s="86"/>
-      <c r="I29" s="87"/>
-      <c r="J29" s="88"/>
+      <c r="B29" s="54"/>
+      <c r="C29" s="66"/>
+      <c r="D29" s="70"/>
+      <c r="E29" s="71"/>
+      <c r="F29" s="72"/>
+      <c r="G29" s="70"/>
+      <c r="H29" s="71"/>
+      <c r="I29" s="72"/>
+      <c r="J29" s="73"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="80">
+      <c r="A30" s="65">
         <v>45009</v>
       </c>
-      <c r="B30" s="69" t="s">
+      <c r="B30" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="81"/>
-      <c r="D30" s="85">
+      <c r="C30" s="66"/>
+      <c r="D30" s="70">
         <v>6</v>
       </c>
-      <c r="E30" s="86">
+      <c r="E30" s="71">
         <v>6.5</v>
       </c>
-      <c r="F30" s="87">
+      <c r="F30" s="72">
         <f>D30*E30</f>
         <v>39</v>
       </c>
-      <c r="G30" s="85">
+      <c r="G30" s="70">
         <v>6.84</v>
       </c>
-      <c r="H30" s="86"/>
-      <c r="I30" s="87"/>
-      <c r="J30" s="88"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="72"/>
+      <c r="J30" s="73"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="80">
+      <c r="A31" s="65">
         <v>45010</v>
       </c>
-      <c r="B31" s="69" t="s">
+      <c r="B31" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="C31" s="81"/>
-      <c r="D31" s="85"/>
-      <c r="E31" s="86"/>
-      <c r="F31" s="87"/>
-      <c r="G31" s="85"/>
-      <c r="H31" s="86"/>
-      <c r="I31" s="87">
+      <c r="C31" s="66"/>
+      <c r="D31" s="70"/>
+      <c r="E31" s="71"/>
+      <c r="F31" s="72"/>
+      <c r="G31" s="70"/>
+      <c r="H31" s="71"/>
+      <c r="I31" s="72">
         <v>95</v>
       </c>
-      <c r="J31" s="88"/>
+      <c r="J31" s="73"/>
     </row>
     <row r="32" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="80">
+      <c r="A32" s="65">
         <v>45011</v>
       </c>
-      <c r="B32" s="69"/>
-      <c r="C32" s="81"/>
-      <c r="D32" s="85"/>
-      <c r="E32" s="86"/>
-      <c r="F32" s="87"/>
-      <c r="G32" s="85"/>
-      <c r="H32" s="86"/>
-      <c r="I32" s="87"/>
-      <c r="J32" s="88"/>
+      <c r="B32" s="54"/>
+      <c r="C32" s="66"/>
+      <c r="D32" s="70"/>
+      <c r="E32" s="71"/>
+      <c r="F32" s="72"/>
+      <c r="G32" s="70"/>
+      <c r="H32" s="71"/>
+      <c r="I32" s="72"/>
+      <c r="J32" s="73"/>
     </row>
     <row r="33" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="103"/>
-      <c r="B33" s="104"/>
-      <c r="C33" s="105">
+      <c r="A33" s="88"/>
+      <c r="B33" s="89"/>
+      <c r="C33" s="90">
         <f>SUM(C4:C32)</f>
         <v>1950</v>
       </c>
-      <c r="D33" s="106">
+      <c r="D33" s="91">
         <f>D3-SUM(D4:D32)</f>
         <v>6</v>
       </c>
-      <c r="E33" s="107"/>
-      <c r="F33" s="108">
+      <c r="E33" s="92"/>
+      <c r="F33" s="93">
         <f>F3-SUM(F4:F32)</f>
         <v>39</v>
       </c>
-      <c r="G33" s="106">
+      <c r="G33" s="91">
         <f>SUM(G4:G32)</f>
         <v>1481.9099999999999</v>
       </c>
-      <c r="H33" s="107">
+      <c r="H33" s="92">
         <f>SUM(H4:H32)</f>
         <v>49</v>
       </c>
-      <c r="I33" s="108">
+      <c r="I33" s="93">
         <f>SUM(I8:I32)</f>
         <v>95</v>
       </c>
-      <c r="J33" s="109">
+      <c r="J33" s="94">
         <f>SUM(J4:J32)</f>
         <v>250</v>
       </c>
@@ -4340,10 +4379,10 @@
     <mergeCell ref="L1:O1"/>
   </mergeCells>
   <conditionalFormatting sqref="O7">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="greaterThan">
       <formula>$O$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="greaterThan">
       <formula>$O$3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4355,8 +4394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4374,883 +4413,883 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="48"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="50" t="s">
+      <c r="E1" s="36"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="51"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="53" t="s">
+      <c r="H1" s="39"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="43"/>
-      <c r="L1" s="54" t="s">
+      <c r="K1" s="31"/>
+      <c r="L1" s="113" t="s">
         <v>78</v>
       </c>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="56"/>
+      <c r="M1" s="114"/>
+      <c r="N1" s="114"/>
+      <c r="O1" s="115"/>
     </row>
     <row r="2" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="57"/>
-      <c r="B2" s="58"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="57" t="s">
+      <c r="A2" s="42"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="60" t="s">
+      <c r="E2" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="61" t="s">
+      <c r="F2" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="63" t="s">
+      <c r="H2" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="64" t="s">
+      <c r="I2" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="J2" s="65"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="57" t="s">
+      <c r="J2" s="50"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="M2" s="115">
+      <c r="M2" s="100">
         <f>D3-(SUM(D4:D35))+'Mese 2'!M2</f>
         <v>20</v>
       </c>
-      <c r="N2" s="66">
+      <c r="N2" s="51"/>
+      <c r="O2" s="52">
         <f>'Mese 1'!F39+F3-(SUM(F4:F35))</f>
         <v>91</v>
       </c>
-      <c r="O2" s="67"/>
     </row>
     <row r="3" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="68"/>
-      <c r="B3" s="69"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="71">
+      <c r="A3" s="53"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="56">
         <v>16</v>
       </c>
-      <c r="E3" s="72">
+      <c r="E3" s="57">
         <v>6.5</v>
       </c>
-      <c r="F3" s="73">
+      <c r="F3" s="58">
         <f>D3*E3</f>
         <v>104</v>
       </c>
-      <c r="G3" s="74"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="74" t="s">
+      <c r="G3" s="59"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="62"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="M3" s="75"/>
-      <c r="N3" s="78"/>
-      <c r="O3" s="79">
+      <c r="M3" s="60"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="64">
         <f>C36*0.1</f>
         <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="80">
+      <c r="A4" s="65">
         <v>45012</v>
       </c>
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="81">
+      <c r="C4" s="66">
         <v>1850</v>
       </c>
-      <c r="D4" s="111"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="87"/>
-      <c r="J4" s="88"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="68" t="s">
+      <c r="D4" s="96"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="M4" s="89"/>
-      <c r="N4" s="69"/>
-      <c r="O4" s="90">
+      <c r="M4" s="74"/>
+      <c r="N4" s="54"/>
+      <c r="O4" s="75">
         <f>G36</f>
         <v>1425.81</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="80">
+      <c r="A5" s="65">
         <v>45013</v>
       </c>
-      <c r="B5" s="69" t="s">
+      <c r="B5" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="81"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="85">
+      <c r="C5" s="66"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="70">
         <v>39.9</v>
       </c>
-      <c r="H5" s="86"/>
-      <c r="I5" s="87"/>
-      <c r="J5" s="88"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="68" t="s">
+      <c r="H5" s="71"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="M5" s="89"/>
-      <c r="N5" s="69"/>
-      <c r="O5" s="90">
+      <c r="M5" s="74"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="75">
         <f>H36</f>
         <v>474</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="80">
+      <c r="A6" s="65">
         <v>45014</v>
       </c>
-      <c r="B6" s="69"/>
-      <c r="C6" s="81"/>
-      <c r="D6" s="112"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="86"/>
-      <c r="I6" s="87"/>
-      <c r="J6" s="88"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="68" t="s">
+      <c r="B6" s="54"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="71"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="73"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="89"/>
-      <c r="N6" s="69"/>
-      <c r="O6" s="90">
+      <c r="M6" s="74"/>
+      <c r="N6" s="54"/>
+      <c r="O6" s="75">
         <f>J36</f>
         <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="80">
+      <c r="A7" s="65">
         <v>45015</v>
       </c>
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="81"/>
-      <c r="D7" s="112"/>
-      <c r="E7" s="86"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="85">
+      <c r="C7" s="66"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="70">
         <v>25</v>
       </c>
-      <c r="H7" s="86"/>
-      <c r="I7" s="87"/>
-      <c r="J7" s="88"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="92" t="s">
+      <c r="H7" s="71"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="M7" s="93"/>
-      <c r="N7" s="94"/>
-      <c r="O7" s="95">
+      <c r="M7" s="78"/>
+      <c r="N7" s="79"/>
+      <c r="O7" s="80">
         <f>C36-G36-J36</f>
         <v>174.19000000000005</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="80">
+      <c r="A8" s="65">
         <v>45016</v>
       </c>
-      <c r="B8" s="69" t="s">
+      <c r="B8" s="54" t="s">
         <v>112</v>
       </c>
-      <c r="C8" s="81"/>
-      <c r="D8" s="112">
+      <c r="C8" s="66"/>
+      <c r="D8" s="97">
         <v>7</v>
       </c>
-      <c r="E8" s="86"/>
-      <c r="F8" s="87">
+      <c r="E8" s="71"/>
+      <c r="F8" s="72">
         <f>D8*E3</f>
         <v>45.5</v>
       </c>
-      <c r="G8" s="85">
+      <c r="G8" s="70">
         <v>24.68</v>
       </c>
-      <c r="H8" s="86"/>
-      <c r="I8" s="87"/>
-      <c r="J8" s="88"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
-      <c r="M8" s="43"/>
-      <c r="N8" s="43"/>
-      <c r="O8" s="43"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="80"/>
-      <c r="B9" s="69" t="s">
+      <c r="A9" s="65"/>
+      <c r="B9" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="81"/>
-      <c r="D9" s="112"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="87"/>
-      <c r="G9" s="85">
+      <c r="C9" s="66"/>
+      <c r="D9" s="97"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="70">
         <v>500</v>
       </c>
-      <c r="H9" s="86"/>
-      <c r="I9" s="87"/>
-      <c r="J9" s="88"/>
-      <c r="K9" s="43"/>
-      <c r="L9" s="43"/>
-      <c r="M9" s="43"/>
-      <c r="N9" s="43"/>
-      <c r="O9" s="43"/>
+      <c r="H9" s="71"/>
+      <c r="I9" s="72"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="80">
+      <c r="A10" s="65">
         <v>45017</v>
       </c>
-      <c r="B10" s="69"/>
-      <c r="C10" s="81"/>
-      <c r="D10" s="112"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="87"/>
-      <c r="G10" s="85"/>
-      <c r="H10" s="86"/>
-      <c r="I10" s="87"/>
-      <c r="J10" s="88"/>
-      <c r="K10" s="43"/>
-      <c r="L10" s="43" t="s">
+      <c r="B10" s="54"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="97"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="70"/>
+      <c r="H10" s="71"/>
+      <c r="I10" s="72"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="M10" s="43"/>
-      <c r="N10" s="43"/>
-      <c r="O10" s="43"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="31"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="80">
+      <c r="A11" s="65">
         <v>45018</v>
       </c>
-      <c r="B11" s="69" t="s">
+      <c r="B11" s="54" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="81"/>
-      <c r="D11" s="112"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="87"/>
-      <c r="G11" s="85">
+      <c r="C11" s="66"/>
+      <c r="D11" s="97"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="72"/>
+      <c r="G11" s="70">
         <v>45</v>
       </c>
-      <c r="H11" s="86"/>
-      <c r="I11" s="87"/>
-      <c r="J11" s="88"/>
-      <c r="K11" s="43"/>
-      <c r="L11" s="43"/>
-      <c r="M11" s="43"/>
-      <c r="N11" s="43"/>
-      <c r="O11" s="43"/>
+      <c r="H11" s="71"/>
+      <c r="I11" s="72"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="80">
+      <c r="A12" s="65">
         <v>45019</v>
       </c>
-      <c r="B12" s="69"/>
-      <c r="C12" s="81"/>
-      <c r="D12" s="112"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="87"/>
-      <c r="G12" s="85"/>
-      <c r="H12" s="86"/>
-      <c r="I12" s="87"/>
-      <c r="J12" s="88"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="43"/>
-      <c r="M12" s="43"/>
-      <c r="N12" s="43"/>
-      <c r="O12" s="43"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="66"/>
+      <c r="D12" s="97"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="72"/>
+      <c r="G12" s="70"/>
+      <c r="H12" s="71"/>
+      <c r="I12" s="72"/>
+      <c r="J12" s="73"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="80">
+      <c r="A13" s="65">
         <v>45020</v>
       </c>
-      <c r="B13" s="69" t="s">
+      <c r="B13" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="C13" s="81"/>
-      <c r="D13" s="112"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="87"/>
-      <c r="G13" s="85">
+      <c r="C13" s="66"/>
+      <c r="D13" s="97"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="70">
         <v>11.92</v>
       </c>
-      <c r="H13" s="86"/>
-      <c r="I13" s="87"/>
-      <c r="J13" s="88"/>
-      <c r="K13" s="43"/>
-      <c r="L13" s="43"/>
-      <c r="M13" s="43"/>
-      <c r="N13" s="43"/>
-      <c r="O13" s="43"/>
+      <c r="H13" s="71"/>
+      <c r="I13" s="72"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="80">
+      <c r="A14" s="65">
         <v>45021</v>
       </c>
-      <c r="B14" s="69" t="s">
+      <c r="B14" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="81"/>
-      <c r="D14" s="112"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="87"/>
-      <c r="G14" s="85"/>
-      <c r="H14" s="86"/>
-      <c r="I14" s="87"/>
-      <c r="J14" s="88">
+      <c r="C14" s="66"/>
+      <c r="D14" s="97"/>
+      <c r="E14" s="71"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="70"/>
+      <c r="H14" s="71"/>
+      <c r="I14" s="72"/>
+      <c r="J14" s="73">
         <v>200</v>
       </c>
-      <c r="K14" s="43"/>
-      <c r="L14" s="43"/>
-      <c r="M14" s="43"/>
-      <c r="N14" s="43"/>
-      <c r="O14" s="43"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="31"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="80">
+      <c r="A15" s="65">
         <v>45022</v>
       </c>
-      <c r="B15" s="69"/>
-      <c r="C15" s="81"/>
-      <c r="D15" s="112"/>
-      <c r="E15" s="86"/>
-      <c r="F15" s="87"/>
-      <c r="G15" s="85"/>
-      <c r="H15" s="86"/>
-      <c r="I15" s="87"/>
-      <c r="J15" s="88"/>
-      <c r="K15" s="43"/>
-      <c r="L15" s="43"/>
-      <c r="M15" s="43"/>
-      <c r="N15" s="43"/>
-      <c r="O15" s="43"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="97"/>
+      <c r="E15" s="71"/>
+      <c r="F15" s="72"/>
+      <c r="G15" s="70"/>
+      <c r="H15" s="71"/>
+      <c r="I15" s="72"/>
+      <c r="J15" s="73"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="31"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="80">
+      <c r="A16" s="65">
         <v>45023</v>
       </c>
-      <c r="B16" s="69"/>
-      <c r="C16" s="81"/>
-      <c r="D16" s="112"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="87"/>
-      <c r="G16" s="85"/>
-      <c r="H16" s="86"/>
-      <c r="I16" s="87"/>
-      <c r="J16" s="88"/>
-      <c r="K16" s="43"/>
-      <c r="L16" s="43"/>
-      <c r="M16" s="43"/>
-      <c r="N16" s="43"/>
-      <c r="O16" s="43"/>
+      <c r="B16" s="54"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="97"/>
+      <c r="E16" s="71"/>
+      <c r="F16" s="72"/>
+      <c r="G16" s="70"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="72"/>
+      <c r="J16" s="73"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="31"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="80">
+      <c r="A17" s="65">
         <v>45024</v>
       </c>
-      <c r="B17" s="69" t="s">
+      <c r="B17" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="C17" s="81"/>
-      <c r="D17" s="112"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="87"/>
-      <c r="G17" s="85"/>
-      <c r="H17" s="86"/>
-      <c r="I17" s="87">
+      <c r="C17" s="66"/>
+      <c r="D17" s="97"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="72"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="72">
         <v>95</v>
       </c>
-      <c r="J17" s="88"/>
-      <c r="K17" s="43"/>
-      <c r="L17" s="43"/>
-      <c r="M17" s="43"/>
-      <c r="N17" s="43"/>
-      <c r="O17" s="43"/>
+      <c r="J17" s="73"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="31"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="80">
+      <c r="A18" s="65">
         <v>45025</v>
       </c>
-      <c r="B18" s="69" t="s">
+      <c r="B18" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="81"/>
-      <c r="D18" s="112"/>
-      <c r="E18" s="86"/>
-      <c r="F18" s="87"/>
-      <c r="G18" s="85">
+      <c r="C18" s="66"/>
+      <c r="D18" s="97"/>
+      <c r="E18" s="71"/>
+      <c r="F18" s="72"/>
+      <c r="G18" s="70">
         <v>30</v>
       </c>
-      <c r="H18" s="86"/>
-      <c r="I18" s="87"/>
-      <c r="J18" s="88"/>
-      <c r="K18" s="43"/>
-      <c r="L18" s="43"/>
-      <c r="M18" s="43"/>
-      <c r="N18" s="43"/>
-      <c r="O18" s="43"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="72"/>
+      <c r="J18" s="73"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="31"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="31"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="80">
+      <c r="A19" s="65">
         <v>45026</v>
       </c>
-      <c r="B19" s="69" t="s">
+      <c r="B19" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="C19" s="81"/>
-      <c r="D19" s="112"/>
-      <c r="E19" s="86"/>
-      <c r="F19" s="87"/>
-      <c r="G19" s="85">
+      <c r="C19" s="66"/>
+      <c r="D19" s="97"/>
+      <c r="E19" s="71"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="70">
         <f>'Mese 2'!H33</f>
         <v>49</v>
       </c>
-      <c r="H19" s="86"/>
-      <c r="I19" s="87"/>
-      <c r="J19" s="88"/>
-      <c r="K19" s="43"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="43"/>
-      <c r="N19" s="43"/>
-      <c r="O19" s="43"/>
+      <c r="H19" s="71"/>
+      <c r="I19" s="72"/>
+      <c r="J19" s="73"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="31"/>
+      <c r="N19" s="31"/>
+      <c r="O19" s="31"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" s="80">
+      <c r="A20" s="65">
         <v>45027</v>
       </c>
-      <c r="B20" s="69" t="s">
+      <c r="B20" s="54" t="s">
         <v>118</v>
       </c>
-      <c r="C20" s="81"/>
-      <c r="D20" s="112"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="87"/>
-      <c r="G20" s="85">
+      <c r="C20" s="66"/>
+      <c r="D20" s="97"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="72"/>
+      <c r="G20" s="70">
         <v>25</v>
       </c>
-      <c r="H20" s="86"/>
-      <c r="I20" s="87"/>
-      <c r="J20" s="88"/>
-      <c r="K20" s="43"/>
-      <c r="L20" s="43"/>
-      <c r="M20" s="43"/>
-      <c r="N20" s="43"/>
-      <c r="O20" s="43"/>
+      <c r="H20" s="71"/>
+      <c r="I20" s="72"/>
+      <c r="J20" s="73"/>
+      <c r="K20" s="31"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="31"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="80">
+      <c r="A21" s="65">
         <v>45028</v>
       </c>
-      <c r="B21" s="69" t="s">
+      <c r="B21" s="54" t="s">
         <v>117</v>
       </c>
-      <c r="C21" s="81"/>
-      <c r="D21" s="112"/>
-      <c r="E21" s="86"/>
-      <c r="F21" s="87"/>
-      <c r="G21" s="85">
+      <c r="C21" s="66"/>
+      <c r="D21" s="97"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="70">
         <v>250</v>
       </c>
-      <c r="H21" s="86"/>
-      <c r="I21" s="87"/>
-      <c r="J21" s="88"/>
-      <c r="K21" s="43"/>
-      <c r="L21" s="43"/>
-      <c r="M21" s="43"/>
-      <c r="N21" s="43"/>
-      <c r="O21" s="43"/>
+      <c r="H21" s="71"/>
+      <c r="I21" s="72"/>
+      <c r="J21" s="73"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="31"/>
+      <c r="M21" s="31"/>
+      <c r="N21" s="31"/>
+      <c r="O21" s="31"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="80">
+      <c r="A22" s="65">
         <v>45029</v>
       </c>
-      <c r="B22" s="69" t="s">
+      <c r="B22" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="81"/>
-      <c r="D22" s="112"/>
-      <c r="E22" s="86"/>
-      <c r="F22" s="87"/>
-      <c r="G22" s="85"/>
-      <c r="H22" s="86">
+      <c r="C22" s="66"/>
+      <c r="D22" s="97"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="70"/>
+      <c r="H22" s="71">
         <v>450</v>
       </c>
-      <c r="I22" s="87"/>
-      <c r="J22" s="88"/>
-      <c r="K22" s="43"/>
-      <c r="L22" s="43"/>
-      <c r="M22" s="43"/>
-      <c r="N22" s="43"/>
-      <c r="O22" s="43"/>
+      <c r="I22" s="72"/>
+      <c r="J22" s="73"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="31"/>
+      <c r="N22" s="31"/>
+      <c r="O22" s="31"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="80">
+      <c r="A23" s="65">
         <v>45030</v>
       </c>
-      <c r="B23" s="69" t="s">
+      <c r="B23" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="C23" s="81"/>
-      <c r="D23" s="112"/>
-      <c r="E23" s="86"/>
-      <c r="F23" s="87"/>
-      <c r="G23" s="85">
+      <c r="C23" s="66"/>
+      <c r="D23" s="97"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="72"/>
+      <c r="G23" s="70">
         <v>18.96</v>
       </c>
-      <c r="H23" s="86"/>
-      <c r="I23" s="87"/>
-      <c r="J23" s="88"/>
-      <c r="K23" s="43"/>
-      <c r="L23" s="43"/>
-      <c r="M23" s="43"/>
-      <c r="N23" s="43"/>
-      <c r="O23" s="43"/>
+      <c r="H23" s="71"/>
+      <c r="I23" s="72"/>
+      <c r="J23" s="73"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="31"/>
+      <c r="N23" s="31"/>
+      <c r="O23" s="31"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="80">
+      <c r="A24" s="65">
         <v>45031</v>
       </c>
-      <c r="B24" s="69" t="s">
+      <c r="B24" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="81"/>
-      <c r="D24" s="112"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="87"/>
-      <c r="G24" s="85">
+      <c r="C24" s="66"/>
+      <c r="D24" s="97"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="72"/>
+      <c r="G24" s="70">
         <v>18</v>
       </c>
-      <c r="H24" s="86"/>
-      <c r="I24" s="87"/>
-      <c r="J24" s="88"/>
-      <c r="K24" s="43"/>
-      <c r="L24" s="43"/>
-      <c r="M24" s="43"/>
-      <c r="N24" s="43"/>
-      <c r="O24" s="43"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="72"/>
+      <c r="J24" s="73"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="31"/>
+      <c r="O24" s="31"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="80">
+      <c r="A25" s="65">
         <v>45032</v>
       </c>
-      <c r="B25" s="69" t="s">
+      <c r="B25" s="54" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="81"/>
-      <c r="D25" s="112"/>
-      <c r="E25" s="86"/>
-      <c r="F25" s="87"/>
-      <c r="G25" s="85">
+      <c r="C25" s="66"/>
+      <c r="D25" s="97"/>
+      <c r="E25" s="71"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="70">
         <v>60</v>
       </c>
-      <c r="H25" s="86"/>
-      <c r="I25" s="87"/>
-      <c r="J25" s="88"/>
-      <c r="K25" s="43"/>
-      <c r="L25" s="43"/>
-      <c r="M25" s="43"/>
-      <c r="N25" s="43"/>
-      <c r="O25" s="43"/>
+      <c r="H25" s="71"/>
+      <c r="I25" s="72"/>
+      <c r="J25" s="73"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="31"/>
+      <c r="N25" s="31"/>
+      <c r="O25" s="31"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="80">
+      <c r="A26" s="65">
         <v>45033</v>
       </c>
-      <c r="B26" s="69"/>
-      <c r="C26" s="81"/>
-      <c r="D26" s="112"/>
-      <c r="E26" s="86"/>
-      <c r="F26" s="87"/>
-      <c r="G26" s="85"/>
-      <c r="H26" s="86"/>
-      <c r="I26" s="87"/>
-      <c r="J26" s="88"/>
-      <c r="K26" s="43"/>
-      <c r="L26" s="43"/>
-      <c r="M26" s="43"/>
-      <c r="N26" s="43"/>
-      <c r="O26" s="43"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="66"/>
+      <c r="D26" s="97"/>
+      <c r="E26" s="71"/>
+      <c r="F26" s="72"/>
+      <c r="G26" s="70"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="72"/>
+      <c r="J26" s="73"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="31"/>
+      <c r="M26" s="31"/>
+      <c r="N26" s="31"/>
+      <c r="O26" s="31"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A27" s="80">
+      <c r="A27" s="65">
         <v>45034</v>
       </c>
-      <c r="B27" s="69" t="s">
+      <c r="B27" s="54" t="s">
         <v>118</v>
       </c>
-      <c r="C27" s="81"/>
-      <c r="D27" s="112"/>
-      <c r="E27" s="86"/>
-      <c r="F27" s="87"/>
-      <c r="G27" s="85">
+      <c r="C27" s="66"/>
+      <c r="D27" s="97"/>
+      <c r="E27" s="71"/>
+      <c r="F27" s="72"/>
+      <c r="G27" s="70">
         <v>45</v>
       </c>
-      <c r="H27" s="86"/>
-      <c r="I27" s="87"/>
-      <c r="J27" s="88"/>
-      <c r="K27" s="43"/>
-      <c r="L27" s="43"/>
-      <c r="M27" s="43"/>
-      <c r="N27" s="43"/>
-      <c r="O27" s="43"/>
+      <c r="H27" s="71"/>
+      <c r="I27" s="72"/>
+      <c r="J27" s="73"/>
+      <c r="K27" s="31"/>
+      <c r="L27" s="31"/>
+      <c r="M27" s="31"/>
+      <c r="N27" s="31"/>
+      <c r="O27" s="31"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A28" s="80">
+      <c r="A28" s="65">
         <v>45035</v>
       </c>
-      <c r="B28" s="69" t="s">
+      <c r="B28" s="54" t="s">
         <v>114</v>
       </c>
-      <c r="C28" s="81"/>
-      <c r="D28" s="112"/>
-      <c r="E28" s="86"/>
-      <c r="F28" s="87"/>
-      <c r="G28" s="85">
+      <c r="C28" s="66"/>
+      <c r="D28" s="97"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="72"/>
+      <c r="G28" s="70">
         <v>30</v>
       </c>
-      <c r="H28" s="86"/>
-      <c r="I28" s="87"/>
-      <c r="J28" s="88"/>
-      <c r="K28" s="43"/>
-      <c r="L28" s="43"/>
-      <c r="M28" s="43"/>
-      <c r="N28" s="43"/>
-      <c r="O28" s="43"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="72"/>
+      <c r="J28" s="73"/>
+      <c r="K28" s="31"/>
+      <c r="L28" s="31"/>
+      <c r="M28" s="31"/>
+      <c r="N28" s="31"/>
+      <c r="O28" s="31"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" s="80">
+      <c r="A29" s="65">
         <v>45036</v>
       </c>
-      <c r="B29" s="69" t="s">
+      <c r="B29" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="81"/>
-      <c r="D29" s="112"/>
-      <c r="E29" s="86"/>
-      <c r="F29" s="87"/>
-      <c r="G29" s="85"/>
-      <c r="H29" s="86"/>
-      <c r="I29" s="87"/>
-      <c r="J29" s="88">
+      <c r="C29" s="66"/>
+      <c r="D29" s="97"/>
+      <c r="E29" s="71"/>
+      <c r="F29" s="72"/>
+      <c r="G29" s="70"/>
+      <c r="H29" s="71"/>
+      <c r="I29" s="72"/>
+      <c r="J29" s="73">
         <v>50</v>
       </c>
-      <c r="K29" s="43"/>
-      <c r="L29" s="43"/>
-      <c r="M29" s="43"/>
-      <c r="N29" s="43"/>
-      <c r="O29" s="43"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="31"/>
+      <c r="M29" s="31"/>
+      <c r="N29" s="31"/>
+      <c r="O29" s="31"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A30" s="80">
+      <c r="A30" s="65">
         <v>45037</v>
       </c>
-      <c r="B30" s="69" t="s">
+      <c r="B30" s="54" t="s">
         <v>115</v>
       </c>
-      <c r="C30" s="81"/>
-      <c r="D30" s="112"/>
-      <c r="E30" s="86"/>
-      <c r="F30" s="87"/>
-      <c r="G30" s="85"/>
-      <c r="H30" s="86">
+      <c r="C30" s="66"/>
+      <c r="D30" s="97"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="72"/>
+      <c r="G30" s="70"/>
+      <c r="H30" s="71">
         <v>24</v>
       </c>
-      <c r="I30" s="87"/>
-      <c r="J30" s="88"/>
-      <c r="K30" s="43"/>
-      <c r="L30" s="43"/>
-      <c r="M30" s="43"/>
-      <c r="N30" s="43"/>
-      <c r="O30" s="43"/>
+      <c r="I30" s="72"/>
+      <c r="J30" s="73"/>
+      <c r="K30" s="31"/>
+      <c r="L30" s="31"/>
+      <c r="M30" s="31"/>
+      <c r="N30" s="31"/>
+      <c r="O30" s="31"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A31" s="80">
+      <c r="A31" s="65">
         <v>45038</v>
       </c>
-      <c r="B31" s="69"/>
-      <c r="C31" s="81"/>
-      <c r="D31" s="112"/>
-      <c r="E31" s="86"/>
-      <c r="F31" s="87"/>
-      <c r="G31" s="85"/>
-      <c r="H31" s="86"/>
-      <c r="I31" s="87"/>
-      <c r="J31" s="88"/>
-      <c r="K31" s="43"/>
-      <c r="L31" s="43"/>
-      <c r="M31" s="43"/>
-      <c r="N31" s="43"/>
-      <c r="O31" s="43"/>
+      <c r="B31" s="54"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="97"/>
+      <c r="E31" s="71"/>
+      <c r="F31" s="72"/>
+      <c r="G31" s="70"/>
+      <c r="H31" s="71"/>
+      <c r="I31" s="72"/>
+      <c r="J31" s="73"/>
+      <c r="K31" s="31"/>
+      <c r="L31" s="31"/>
+      <c r="M31" s="31"/>
+      <c r="N31" s="31"/>
+      <c r="O31" s="31"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A32" s="80">
+      <c r="A32" s="65">
         <v>45039</v>
       </c>
-      <c r="B32" s="69" t="s">
+      <c r="B32" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="C32" s="81"/>
-      <c r="D32" s="112"/>
-      <c r="E32" s="86"/>
-      <c r="F32" s="87"/>
-      <c r="G32" s="85">
+      <c r="C32" s="66"/>
+      <c r="D32" s="97"/>
+      <c r="E32" s="71"/>
+      <c r="F32" s="72"/>
+      <c r="G32" s="70">
         <v>30</v>
       </c>
-      <c r="H32" s="86"/>
-      <c r="I32" s="87"/>
-      <c r="J32" s="88"/>
-      <c r="K32" s="43"/>
-      <c r="L32" s="43"/>
-      <c r="M32" s="43"/>
-      <c r="N32" s="43"/>
-      <c r="O32" s="43"/>
+      <c r="H32" s="71"/>
+      <c r="I32" s="72"/>
+      <c r="J32" s="73"/>
+      <c r="K32" s="31"/>
+      <c r="L32" s="31"/>
+      <c r="M32" s="31"/>
+      <c r="N32" s="31"/>
+      <c r="O32" s="31"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A33" s="80">
+      <c r="A33" s="65">
         <v>45040</v>
       </c>
-      <c r="B33" s="69" t="s">
+      <c r="B33" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="81"/>
-      <c r="D33" s="112"/>
-      <c r="E33" s="86"/>
-      <c r="F33" s="87"/>
-      <c r="G33" s="85">
+      <c r="C33" s="66"/>
+      <c r="D33" s="97"/>
+      <c r="E33" s="71"/>
+      <c r="F33" s="72"/>
+      <c r="G33" s="70">
         <v>108</v>
       </c>
-      <c r="H33" s="86"/>
-      <c r="I33" s="87"/>
-      <c r="J33" s="88"/>
-      <c r="K33" s="43"/>
-      <c r="L33" s="43"/>
-      <c r="M33" s="43"/>
-      <c r="N33" s="43"/>
-      <c r="O33" s="43"/>
+      <c r="H33" s="71"/>
+      <c r="I33" s="72"/>
+      <c r="J33" s="73"/>
+      <c r="K33" s="31"/>
+      <c r="L33" s="31"/>
+      <c r="M33" s="31"/>
+      <c r="N33" s="31"/>
+      <c r="O33" s="31"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A34" s="80">
+      <c r="A34" s="65">
         <v>45041</v>
       </c>
-      <c r="B34" s="69" t="s">
+      <c r="B34" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="C34" s="81"/>
-      <c r="D34" s="112"/>
-      <c r="E34" s="86"/>
-      <c r="F34" s="87"/>
-      <c r="G34" s="85">
+      <c r="C34" s="66"/>
+      <c r="D34" s="97"/>
+      <c r="E34" s="71"/>
+      <c r="F34" s="72"/>
+      <c r="G34" s="70">
         <v>47.35</v>
       </c>
-      <c r="H34" s="86"/>
-      <c r="I34" s="87"/>
-      <c r="J34" s="88"/>
-      <c r="K34" s="43"/>
-      <c r="L34" s="43"/>
-      <c r="M34" s="43"/>
-      <c r="N34" s="43"/>
-      <c r="O34" s="43"/>
+      <c r="H34" s="71"/>
+      <c r="I34" s="72"/>
+      <c r="J34" s="73"/>
+      <c r="K34" s="31"/>
+      <c r="L34" s="31"/>
+      <c r="M34" s="31"/>
+      <c r="N34" s="31"/>
+      <c r="O34" s="31"/>
     </row>
     <row r="35" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="80">
+      <c r="A35" s="65">
         <v>45042</v>
       </c>
-      <c r="B35" s="69" t="s">
+      <c r="B35" s="54" t="s">
         <v>118</v>
       </c>
-      <c r="C35" s="81"/>
-      <c r="D35" s="112"/>
-      <c r="E35" s="86"/>
-      <c r="F35" s="87"/>
-      <c r="G35" s="85">
+      <c r="C35" s="66"/>
+      <c r="D35" s="97"/>
+      <c r="E35" s="71"/>
+      <c r="F35" s="72"/>
+      <c r="G35" s="70">
         <v>68</v>
       </c>
-      <c r="H35" s="86"/>
-      <c r="I35" s="87"/>
-      <c r="J35" s="88"/>
-      <c r="K35" s="43"/>
-      <c r="L35" s="43"/>
-      <c r="M35" s="43"/>
-      <c r="N35" s="43"/>
-      <c r="O35" s="43"/>
+      <c r="H35" s="71"/>
+      <c r="I35" s="72"/>
+      <c r="J35" s="73"/>
+      <c r="K35" s="31"/>
+      <c r="L35" s="31"/>
+      <c r="M35" s="31"/>
+      <c r="N35" s="31"/>
+      <c r="O35" s="31"/>
     </row>
     <row r="36" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="103"/>
-      <c r="B36" s="104"/>
-      <c r="C36" s="105">
+      <c r="A36" s="88"/>
+      <c r="B36" s="89"/>
+      <c r="C36" s="90">
         <f>SUM(C4:C35)</f>
         <v>1850</v>
       </c>
-      <c r="D36" s="114">
+      <c r="D36" s="99">
         <f>SUM(D4:D35)</f>
         <v>7</v>
       </c>
-      <c r="E36" s="105">
+      <c r="E36" s="90">
         <f t="shared" ref="E36:J36" si="0">SUM(E4:E35)</f>
         <v>0</v>
       </c>
-      <c r="F36" s="106">
+      <c r="F36" s="91">
         <f t="shared" si="0"/>
         <v>45.5</v>
       </c>
-      <c r="G36" s="105">
+      <c r="G36" s="90">
         <f t="shared" si="0"/>
         <v>1425.81</v>
       </c>
-      <c r="H36" s="106">
+      <c r="H36" s="91">
         <f t="shared" si="0"/>
         <v>474</v>
       </c>
-      <c r="I36" s="105">
+      <c r="I36" s="90">
         <f t="shared" si="0"/>
         <v>95</v>
       </c>
-      <c r="J36" s="106">
+      <c r="J36" s="91">
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
-      <c r="K36" s="43"/>
-      <c r="L36" s="43"/>
-      <c r="M36" s="43"/>
-      <c r="N36" s="43"/>
-      <c r="O36" s="43"/>
+      <c r="K36" s="31"/>
+      <c r="L36" s="31"/>
+      <c r="M36" s="31"/>
+      <c r="N36" s="31"/>
+      <c r="O36" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="L1:O1"/>
   </mergeCells>
   <conditionalFormatting sqref="O7">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="lessThan">
       <formula>$O$3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>